<commit_message>
adding 1600 MWe extra NGCC capacity for testing
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA487C56-3E2E-4297-B3A1-95DCC806B40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D98A369-2224-4D8C-B999-787BFD14F1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,6 +496,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1023,7 +1024,7 @@
   <dimension ref="A1:BD7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1483,7 +1484,7 @@
         <v>75</v>
       </c>
       <c r="I5">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J5" s="9">
         <v>200</v>

</xml_diff>

<commit_message>
new input files, some of which are broken
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D98A369-2224-4D8C-B999-787BFD14F1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6980351-D558-4020-963B-B64269FF0E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="133">
   <si>
     <t>Setting</t>
   </si>
@@ -283,145 +283,160 @@
     <t>1_nuclear_1</t>
   </si>
   <si>
-    <t>Tech10</t>
-  </si>
-  <si>
-    <t>Nuclear_adv</t>
-  </si>
-  <si>
     <t>Nuclear</t>
   </si>
   <si>
+    <t>bus_name</t>
+  </si>
+  <si>
+    <t>baseKV</t>
+  </si>
+  <si>
+    <t>bus type</t>
+  </si>
+  <si>
+    <t>MW load</t>
+  </si>
+  <si>
+    <t>MVAR load</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>sub area</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>EAS_market_zone</t>
+  </si>
+  <si>
+    <t>ERCOT</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>f_bus</t>
+  </si>
+  <si>
+    <t>t_bus</t>
+  </si>
+  <si>
+    <t>br_r</t>
+  </si>
+  <si>
+    <t>br_x</t>
+  </si>
+  <si>
+    <t>br_b</t>
+  </si>
+  <si>
+    <t>rate_a</t>
+  </si>
+  <si>
+    <t>rate_b</t>
+  </si>
+  <si>
+    <t>rate_c</t>
+  </si>
+  <si>
+    <t>Perm OutRate</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Tr Ratio</t>
+  </si>
+  <si>
+    <t>Tran OutRate</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>model_flag</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>sub_area_i</t>
+  </si>
+  <si>
+    <t>sub_area_1</t>
+  </si>
+  <si>
+    <t>1_storage_1</t>
+  </si>
+  <si>
+    <t>Tech1</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Tech4</t>
+  </si>
+  <si>
+    <t>1_coal_1</t>
+  </si>
+  <si>
+    <t>Tech5</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>ConventionalNuclear</t>
+  </si>
+  <si>
     <t>AdvancedNuclear</t>
   </si>
   <si>
-    <t>bus_name</t>
-  </si>
-  <si>
-    <t>baseKV</t>
-  </si>
-  <si>
-    <t>bus type</t>
-  </si>
-  <si>
-    <t>MW load</t>
-  </si>
-  <si>
-    <t>MVAR load</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>sub area</t>
-  </si>
-  <si>
-    <t>zone</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lng</t>
-  </si>
-  <si>
-    <t>EAS_market_zone</t>
-  </si>
-  <si>
-    <t>ERCOT</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>UID</t>
-  </si>
-  <si>
-    <t>f_bus</t>
-  </si>
-  <si>
-    <t>t_bus</t>
-  </si>
-  <si>
-    <t>br_r</t>
-  </si>
-  <si>
-    <t>br_x</t>
-  </si>
-  <si>
-    <t>br_b</t>
-  </si>
-  <si>
-    <t>rate_a</t>
-  </si>
-  <si>
-    <t>rate_b</t>
-  </si>
-  <si>
-    <t>rate_c</t>
-  </si>
-  <si>
-    <t>Perm OutRate</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Tr Ratio</t>
-  </si>
-  <si>
-    <t>Tran OutRate</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>model_flag</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>sub_area_i</t>
-  </si>
-  <si>
-    <t>sub_area_1</t>
-  </si>
-  <si>
-    <t>1_storage_1</t>
-  </si>
-  <si>
-    <t>Tech1</t>
-  </si>
-  <si>
-    <t>STORAGE</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Tech4</t>
-  </si>
-  <si>
-    <t>1_coal_1</t>
-  </si>
-  <si>
-    <t>Tech5</t>
-  </si>
-  <si>
-    <t>COAL</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Steam</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>CT</t>
+    <t>1_nuclear_A</t>
+  </si>
+  <si>
+    <t>1_nuclear_C</t>
+  </si>
+  <si>
+    <t>UNITGROUP</t>
+  </si>
+  <si>
+    <t>UNIT_CATEGORY</t>
+  </si>
+  <si>
+    <t>UNIT_TYPE</t>
+  </si>
+  <si>
+    <t>FUEL</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,6 +513,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -536,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -622,6 +643,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -636,7 +668,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,6 +703,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1021,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BD7"/>
+  <dimension ref="A1:BD8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E1" sqref="E1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1036,7 +1071,7 @@
     <col min="11" max="12" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="75.75" customHeight="1">
+    <row r="1" spans="1:56" ht="75.75" customHeight="1" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1049,22 +1084,22 @@
       <c r="D1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="E1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="14" t="s">
@@ -1214,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1238,7 +1273,7 @@
         <v>100</v>
       </c>
       <c r="K2" s="12">
-        <v>99999999</v>
+        <v>0</v>
       </c>
       <c r="L2" s="12">
         <v>0</v>
@@ -1246,7 +1281,6 @@
       <c r="M2" s="12">
         <v>0</v>
       </c>
-      <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
@@ -1298,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -1322,7 +1356,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="12">
-        <v>99999999</v>
+        <v>0</v>
       </c>
       <c r="L3" s="12">
         <v>0</v>
@@ -1330,7 +1364,6 @@
       <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
@@ -1376,28 +1409,28 @@
     </row>
     <row r="4" spans="1:56">
       <c r="A4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I4">
         <v>19</v>
@@ -1406,7 +1439,7 @@
         <v>500</v>
       </c>
       <c r="K4" s="12">
-        <v>99999999</v>
+        <v>0</v>
       </c>
       <c r="L4" s="12">
         <v>0</v>
@@ -1414,7 +1447,6 @@
       <c r="M4" s="12">
         <v>0</v>
       </c>
-      <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -1466,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1484,13 +1516,13 @@
         <v>75</v>
       </c>
       <c r="I5">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J5" s="9">
         <v>200</v>
       </c>
       <c r="K5" s="12">
-        <v>99999999</v>
+        <v>0</v>
       </c>
       <c r="L5" s="12">
         <v>0</v>
@@ -1498,7 +1530,6 @@
       <c r="M5" s="12">
         <v>0</v>
       </c>
-      <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -1550,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -1574,7 +1605,7 @@
         <v>50</v>
       </c>
       <c r="K6" s="12">
-        <v>99999999</v>
+        <v>0</v>
       </c>
       <c r="L6" s="12">
         <v>0</v>
@@ -1582,7 +1613,6 @@
       <c r="M6" s="12">
         <v>0</v>
       </c>
-      <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -1628,46 +1658,88 @@
     </row>
     <row r="7" spans="1:56">
       <c r="A7" s="6" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="I7">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="J7" s="9">
+        <v>1050</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56">
+      <c r="A8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
         <v>300</v>
       </c>
-      <c r="K7" s="12">
-        <v>99999999</v>
-      </c>
-      <c r="L7" s="12">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12">
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="12">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1692,37 +1764,37 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1730,13 +1802,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="6">
         <v>345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E2" s="6">
         <v>89177</v>
@@ -1813,54 +1885,54 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -1960,28 +2032,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1989,13 +2061,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="6">
         <v>345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -2043,7 +2115,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2247,28 +2319,28 @@
     </row>
     <row r="2" spans="1:56">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
         <v>116</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" t="s">
-        <v>119</v>
-      </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2376,22 +2448,22 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -2411,28 +2483,28 @@
     </row>
     <row r="6" spans="1:56">
       <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
         <v>121</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>122</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" t="s">
-        <v>125</v>
-      </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I6">
         <v>29</v>
@@ -2470,7 +2542,7 @@
         <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H7" t="s">
         <v>75</v>
@@ -2511,7 +2583,7 @@
         <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H8" t="s">
         <v>75</v>
@@ -2552,7 +2624,7 @@
         <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H9" t="s">
         <v>75</v>
@@ -2593,7 +2665,7 @@
         <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s">
         <v>75</v>
@@ -2634,7 +2706,7 @@
         <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
updating input data files
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_IL.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_IL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6980351-D558-4020-963B-B64269FF0E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02DEE72-D5F7-43B7-A848-A91AE8BE8A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case setting" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="134">
   <si>
     <t>Setting</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>FUEL</t>
+  </si>
+  <si>
+    <t>INITIAL</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,19 +511,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,6 +550,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,17 +638,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,12 +653,12 @@
         <color theme="8"/>
       </top>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39994506668294322"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
@@ -667,8 +670,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -701,25 +712,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="17" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="17" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="19">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
+    <cellStyle name="20% - Accent4 2" xfId="15" xr:uid="{A8E5EF67-AED8-40DC-AA2A-05A7BBD35018}"/>
     <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 2 2" xfId="13" xr:uid="{F533DCFF-9E11-4ABD-8464-1F2D667B7827}"/>
     <cellStyle name="Currency 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Currency 2 2" xfId="12" xr:uid="{0AE19EE1-F265-4D6E-A79B-356956B53BC0}"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
+    <cellStyle name="Heading 2 2" xfId="18" xr:uid="{8099B2DC-6DC0-400A-8DD5-BC4AB8456ACA}"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Heading 3 2" xfId="17" xr:uid="{D08823F0-1667-49EB-8FAC-96AF33A56D51}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2" xfId="11" xr:uid="{ABA552E9-6E59-4136-95DD-51E3F5AD7D96}"/>
     <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 4 2" xfId="14" xr:uid="{CDB9CAD7-571F-47F2-9D97-7457E9E5832B}"/>
     <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21"/>
+    <cellStyle name="Output 2" xfId="16" xr:uid="{3C1F8A8E-29C6-485F-8FDB-A46DBE5EE392}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1059,7 +1081,7 @@
   <dimension ref="A1:BD8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J1"/>
+      <selection sqref="A1:BD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1078,41 +1100,41 @@
       <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>20</v>
@@ -1739,7 +1761,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>